<commit_message>
Fix typo in column names
</commit_message>
<xml_diff>
--- a/data/data2022.xlsx
+++ b/data/data2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/136717c044a40174/Documents/CodeDevelopment/finding-the-mole/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="8_{ABCA4068-F7CE-4E56-BCA6-4C11A5F0FC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD1648C0-C822-4F0E-8FED-89F2F0C03CDF}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="8_{ABCA4068-F7CE-4E56-BCA6-4C11A5F0FC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DB4753E-E8AF-4A76-A99C-CD884306A446}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{6C77B9D9-B416-4DCC-B0D1-B5575DB87CA0}"/>
+    <workbookView xWindow="0" yWindow="84" windowWidth="17280" windowHeight="8880" xr2:uid="{6C77B9D9-B416-4DCC-B0D1-B5575DB87CA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,91 +80,91 @@
     <t>Welmoed</t>
   </si>
   <si>
-    <t>TasP1</t>
-  </si>
-  <si>
-    <t>TasP2</t>
-  </si>
-  <si>
-    <t>TasP3</t>
-  </si>
-  <si>
-    <t>TasP4</t>
-  </si>
-  <si>
-    <t>TasP5</t>
-  </si>
-  <si>
-    <t>TasP6</t>
-  </si>
-  <si>
-    <t>TasP7</t>
-  </si>
-  <si>
-    <t>TasP8</t>
-  </si>
-  <si>
-    <t>TasP9</t>
-  </si>
-  <si>
-    <t>TasP10</t>
-  </si>
-  <si>
-    <t>TasP11</t>
-  </si>
-  <si>
-    <t>TasP12</t>
-  </si>
-  <si>
-    <t>TasP13</t>
-  </si>
-  <si>
-    <t>TasP14</t>
-  </si>
-  <si>
-    <t>TasP15</t>
-  </si>
-  <si>
-    <t>TasP16</t>
-  </si>
-  <si>
-    <t>TasP17</t>
-  </si>
-  <si>
-    <t>TasP18</t>
-  </si>
-  <si>
-    <t>TasP19</t>
-  </si>
-  <si>
-    <t>TasP20</t>
-  </si>
-  <si>
-    <t>TasP21</t>
-  </si>
-  <si>
-    <t>TasP22</t>
-  </si>
-  <si>
-    <t>TasP23</t>
-  </si>
-  <si>
-    <t>TasP24</t>
-  </si>
-  <si>
-    <t>TasP25</t>
-  </si>
-  <si>
-    <t>TasP26</t>
-  </si>
-  <si>
-    <t>TasP27</t>
-  </si>
-  <si>
     <t>P</t>
   </si>
   <si>
     <t>Pim-Lian</t>
+  </si>
+  <si>
+    <t>Task1</t>
+  </si>
+  <si>
+    <t>Task2</t>
+  </si>
+  <si>
+    <t>Task3</t>
+  </si>
+  <si>
+    <t>Task4</t>
+  </si>
+  <si>
+    <t>Task5</t>
+  </si>
+  <si>
+    <t>Task6</t>
+  </si>
+  <si>
+    <t>Task7</t>
+  </si>
+  <si>
+    <t>Task8</t>
+  </si>
+  <si>
+    <t>Task9</t>
+  </si>
+  <si>
+    <t>Task10</t>
+  </si>
+  <si>
+    <t>Task11</t>
+  </si>
+  <si>
+    <t>Task12</t>
+  </si>
+  <si>
+    <t>Task13</t>
+  </si>
+  <si>
+    <t>Task14</t>
+  </si>
+  <si>
+    <t>Task15</t>
+  </si>
+  <si>
+    <t>Task16</t>
+  </si>
+  <si>
+    <t>Task17</t>
+  </si>
+  <si>
+    <t>Task18</t>
+  </si>
+  <si>
+    <t>Task19</t>
+  </si>
+  <si>
+    <t>Task20</t>
+  </si>
+  <si>
+    <t>Task21</t>
+  </si>
+  <si>
+    <t>Task22</t>
+  </si>
+  <si>
+    <t>Task23</t>
+  </si>
+  <si>
+    <t>Task24</t>
+  </si>
+  <si>
+    <t>Task25</t>
+  </si>
+  <si>
+    <t>Task26</t>
+  </si>
+  <si>
+    <t>Task27</t>
   </si>
 </sst>
 </file>
@@ -524,7 +524,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="X4" sqref="A1:AB12"/>
+      <selection pane="topRight" activeCell="S4" sqref="A1:AB12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -534,85 +534,85 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="M1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="N1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="O1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="P1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="R1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="S1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="T1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="U1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="V1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="W1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="X1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="Y1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="Z1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="AA1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="AB1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
@@ -620,7 +620,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -632,13 +632,13 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
         <v>3</v>
       </c>
       <c r="H2" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="I2" t="s">
         <v>2</v>
@@ -718,7 +718,7 @@
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
         <v>3</v>
@@ -757,7 +757,7 @@
         <v>2</v>
       </c>
       <c r="S3" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="T3" t="s">
         <v>2</v>
@@ -801,7 +801,7 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
         <v>3</v>
@@ -810,7 +810,7 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="I4" t="s">
         <v>2</v>
@@ -858,7 +858,7 @@
         <v>2</v>
       </c>
       <c r="X4" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="Y4" t="s">
         <v>2</v>
@@ -887,7 +887,7 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
         <v>3</v>
@@ -964,7 +964,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -973,7 +973,7 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="F6" t="s">
         <v>3</v>
@@ -982,7 +982,7 @@
         <v>3</v>
       </c>
       <c r="H6" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="I6" t="s">
         <v>2</v>
@@ -1047,7 +1047,7 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -1065,10 +1065,10 @@
         <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="H7" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="I7" t="s">
         <v>2</v>
@@ -1095,7 +1095,7 @@
         <v>2</v>
       </c>
       <c r="Q7" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="R7" t="s">
         <v>2</v>
@@ -1116,7 +1116,7 @@
         <v>2</v>
       </c>
       <c r="X7" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="Y7" t="s">
         <v>2</v>
@@ -1136,7 +1136,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -1145,13 +1145,13 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="F8" t="s">
         <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="H8" t="s">
         <v>3</v>
@@ -1240,7 +1240,7 @@
         <v>3</v>
       </c>
       <c r="H9" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="I9" t="s">
         <v>2</v>
@@ -1267,7 +1267,7 @@
         <v>2</v>
       </c>
       <c r="Q9" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="R9" t="s">
         <v>2</v>
@@ -1308,7 +1308,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
@@ -1394,7 +1394,7 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -1409,7 +1409,7 @@
         <v>3</v>
       </c>
       <c r="G11" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="H11" t="s">
         <v>3</v>
@@ -1433,13 +1433,13 @@
         <v>2</v>
       </c>
       <c r="O11" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="P11" t="s">
         <v>2</v>
       </c>
       <c r="Q11" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="R11" t="s">
         <v>2</v>
@@ -1480,7 +1480,7 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -1489,7 +1489,7 @@
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="F12" t="s">
         <v>3</v>
@@ -1498,7 +1498,7 @@
         <v>3</v>
       </c>
       <c r="H12" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="I12" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Fix typo in name
</commit_message>
<xml_diff>
--- a/data/data2022.xlsx
+++ b/data/data2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/136717c044a40174/Documents/CodeDevelopment/finding-the-mole/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="98" documentId="8_{ABCA4068-F7CE-4E56-BCA6-4C11A5F0FC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DB4753E-E8AF-4A76-A99C-CD884306A446}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="8_{ABCA4068-F7CE-4E56-BCA6-4C11A5F0FC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{079FF0BB-7E40-43F4-8678-319B0D23F1BE}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="84" windowWidth="17280" windowHeight="8880" xr2:uid="{6C77B9D9-B416-4DCC-B0D1-B5575DB87CA0}"/>
   </bookViews>
@@ -83,9 +83,6 @@
     <t>P</t>
   </si>
   <si>
-    <t>Pim-Lian</t>
-  </si>
-  <si>
     <t>Task1</t>
   </si>
   <si>
@@ -165,6 +162,9 @@
   </si>
   <si>
     <t>Task27</t>
+  </si>
+  <si>
+    <t>Kim-Lian</t>
   </si>
 </sst>
 </file>
@@ -524,7 +524,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S4" sqref="A1:AB12"/>
+      <selection pane="topRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -534,85 +534,85 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>24</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>25</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>26</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>27</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>28</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>29</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>31</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>32</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>33</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>34</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>35</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>36</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>37</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>38</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>39</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>40</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>41</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
@@ -1047,7 +1047,7 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>

</xml_diff>